<commit_message>
add 1999 time window in some files
</commit_message>
<xml_diff>
--- a/Test/DocNum&density.xlsx
+++ b/Test/DocNum&density.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="DocNum&amp;density" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -969,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -999,587 +999,652 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="J6" s="1">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1">
+        <v>42</v>
+      </c>
+      <c r="F7" s="1">
+        <v>68</v>
+      </c>
+      <c r="G7" s="1">
         <v>79</v>
-      </c>
-      <c r="B7" s="1">
-        <v>107</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44</v>
-      </c>
-      <c r="D7" s="1">
-        <v>50</v>
-      </c>
-      <c r="E7" s="1">
-        <v>43</v>
-      </c>
-      <c r="F7" s="1">
-        <v>81</v>
-      </c>
-      <c r="G7" s="1">
-        <v>78</v>
       </c>
       <c r="H7" s="1">
         <v>65</v>
       </c>
       <c r="I7" s="1">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="J7" s="1">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
+        <v>79</v>
+      </c>
+      <c r="B8" s="1">
+        <v>107</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44</v>
+      </c>
+      <c r="D8" s="1">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1">
+        <v>43</v>
+      </c>
+      <c r="F8" s="1">
+        <v>81</v>
+      </c>
+      <c r="G8" s="1">
         <v>78</v>
       </c>
-      <c r="B8" s="1">
-        <v>31</v>
-      </c>
-      <c r="C8" s="1">
-        <v>91</v>
-      </c>
-      <c r="D8" s="1">
-        <v>62</v>
-      </c>
-      <c r="E8" s="1">
-        <v>127</v>
-      </c>
-      <c r="F8" s="1">
-        <v>148</v>
-      </c>
-      <c r="G8" s="1">
-        <v>63</v>
-      </c>
       <c r="H8" s="1">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="I8" s="1">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="J8" s="1">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <v>132</v>
+        <v>78</v>
       </c>
       <c r="B9" s="1">
-        <v>198</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1">
-        <v>121</v>
+        <v>62</v>
       </c>
       <c r="E9" s="1">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="F9" s="1">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="G9" s="1">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="H9" s="1">
-        <v>139</v>
+        <v>36</v>
       </c>
       <c r="I9" s="1">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="J9" s="1">
-        <v>210</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <v>255</v>
+        <v>132</v>
       </c>
       <c r="B10" s="1">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C10" s="1">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D10" s="1">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E10" s="1">
-        <v>256</v>
+        <v>179</v>
       </c>
       <c r="F10" s="1">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="G10" s="1">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="H10" s="1">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="I10" s="1">
-        <v>198</v>
+        <v>122</v>
       </c>
       <c r="J10" s="1">
-        <v>133</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
-        <v>192</v>
+        <v>255</v>
       </c>
       <c r="B11" s="1">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="C11" s="1">
-        <v>158</v>
+        <v>105</v>
       </c>
       <c r="D11" s="1">
-        <v>173</v>
+        <v>133</v>
       </c>
       <c r="E11" s="1">
-        <v>150</v>
+        <v>256</v>
       </c>
       <c r="F11" s="1">
-        <v>141</v>
+        <v>218</v>
       </c>
       <c r="G11" s="1">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="H11" s="1">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="I11" s="1">
-        <v>137</v>
+        <v>198</v>
       </c>
       <c r="J11" s="1">
-        <v>170</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="B12" s="1">
-        <v>284</v>
+        <v>174</v>
       </c>
       <c r="C12" s="1">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="D12" s="1">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="E12" s="1">
-        <v>225</v>
+        <v>150</v>
       </c>
       <c r="F12" s="1">
-        <v>325</v>
+        <v>141</v>
       </c>
       <c r="G12" s="1">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="H12" s="1">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="I12" s="1">
-        <v>284</v>
+        <v>137</v>
       </c>
       <c r="J12" s="1">
-        <v>299</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="B13" s="1">
-        <v>156</v>
+        <v>284</v>
       </c>
       <c r="C13" s="1">
-        <v>211</v>
+        <v>82</v>
       </c>
       <c r="D13" s="1">
-        <v>265</v>
+        <v>157</v>
       </c>
       <c r="E13" s="1">
-        <v>289</v>
+        <v>225</v>
       </c>
       <c r="F13" s="1">
-        <v>207</v>
+        <v>325</v>
       </c>
       <c r="G13" s="1">
-        <v>361</v>
+        <v>199</v>
       </c>
       <c r="H13" s="1">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="I13" s="1">
-        <v>178</v>
+        <v>284</v>
       </c>
       <c r="J13" s="1">
-        <v>254</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
+        <v>109</v>
+      </c>
+      <c r="B14" s="1">
+        <v>156</v>
+      </c>
+      <c r="C14" s="1">
+        <v>211</v>
+      </c>
+      <c r="D14" s="1">
+        <v>265</v>
+      </c>
+      <c r="E14" s="1">
+        <v>289</v>
+      </c>
+      <c r="F14" s="1">
+        <v>207</v>
+      </c>
+      <c r="G14" s="1">
+        <v>361</v>
+      </c>
+      <c r="H14" s="1">
+        <v>180</v>
+      </c>
+      <c r="I14" s="1">
+        <v>178</v>
+      </c>
+      <c r="J14" s="1">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
         <v>76</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <v>105</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C15" s="1">
         <v>93</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <v>52</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E15" s="1">
         <v>43</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F15" s="1">
         <v>96</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G15" s="1">
         <v>123</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H15" s="1">
         <v>45</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I15" s="1">
         <v>151</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J15" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="1">
-        <v>1.6712865259740199</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1.6515280032467501</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1.5558705357142799</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1.59272930194805</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1.6356838474025901</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1.66725649350649</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1.6981067370129801</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1.64132508116883</v>
-      </c>
-      <c r="I17" s="1">
-        <v>1.6191761363636299</v>
-      </c>
-      <c r="J17" s="1">
-        <v>1.62285511363636</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
-        <v>1.89232142857142</v>
+        <v>0.505390963203463</v>
       </c>
       <c r="B18" s="1">
-        <v>1.8803733766233699</v>
+        <v>0.41127232142857101</v>
       </c>
       <c r="C18" s="1">
-        <v>1.8735978084415501</v>
+        <v>0.43736810064935</v>
       </c>
       <c r="D18" s="1">
-        <v>1.83980722402597</v>
+        <v>0.510545183982684</v>
       </c>
       <c r="E18" s="1">
-        <v>1.83252435064935</v>
+        <v>0.50582724567099502</v>
       </c>
       <c r="F18" s="1">
-        <v>1.9428409090909</v>
+        <v>0.49897186147186101</v>
       </c>
       <c r="G18" s="1">
-        <v>1.84422280844155</v>
+        <v>0.432359307359307</v>
       </c>
       <c r="H18" s="1">
-        <v>1.8115259740259699</v>
+        <v>0.49975311147186102</v>
       </c>
       <c r="I18" s="1">
-        <v>1.8386140422077899</v>
+        <v>0.46702178030302999</v>
       </c>
       <c r="J18" s="1">
-        <v>1.7873336038961001</v>
+        <v>0.54040178571428499</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
-        <v>2.1872646103896098</v>
+        <v>1.6712865259740199</v>
       </c>
       <c r="B19" s="1">
-        <v>2.0861952110389601</v>
+        <v>1.6515280032467501</v>
       </c>
       <c r="C19" s="1">
-        <v>2.2295008116883102</v>
+        <v>1.5558705357142799</v>
       </c>
       <c r="D19" s="1">
-        <v>2.1416883116883101</v>
+        <v>1.59272930194805</v>
       </c>
       <c r="E19" s="1">
-        <v>2.1707061688311602</v>
+        <v>1.6356838474025901</v>
       </c>
       <c r="F19" s="1">
-        <v>2.2177130681818098</v>
+        <v>1.66725649350649</v>
       </c>
       <c r="G19" s="1">
-        <v>2.1811566558441502</v>
+        <v>1.6981067370129801</v>
       </c>
       <c r="H19" s="1">
-        <v>2.0572098214285699</v>
+        <v>1.64132508116883</v>
       </c>
       <c r="I19" s="1">
-        <v>2.2027962662337601</v>
+        <v>1.6191761363636299</v>
       </c>
       <c r="J19" s="1">
-        <v>2.1981107954545398</v>
+        <v>1.62285511363636</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
-        <v>4.5917816558441498</v>
+        <v>1.89232142857142</v>
       </c>
       <c r="B20" s="1">
-        <v>4.5945556006493504</v>
+        <v>1.8803733766233699</v>
       </c>
       <c r="C20" s="1">
-        <v>4.7019825487012898</v>
+        <v>1.8735978084415501</v>
       </c>
       <c r="D20" s="1">
-        <v>4.60002232142857</v>
+        <v>1.83980722402597</v>
       </c>
       <c r="E20" s="1">
-        <v>4.7393344155844099</v>
+        <v>1.83252435064935</v>
       </c>
       <c r="F20" s="1">
-        <v>4.6667167207792097</v>
+        <v>1.9428409090909</v>
       </c>
       <c r="G20" s="1">
-        <v>4.4920880681818103</v>
+        <v>1.84422280844155</v>
       </c>
       <c r="H20" s="1">
-        <v>4.5418486201298602</v>
+        <v>1.8115259740259699</v>
       </c>
       <c r="I20" s="1">
-        <v>4.4995616883116902</v>
+        <v>1.8386140422077899</v>
       </c>
       <c r="J20" s="1">
-        <v>4.73885551948052</v>
+        <v>1.7873336038961001</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
-        <v>5.5341112012986997</v>
+        <v>2.1872646103896098</v>
       </c>
       <c r="B21" s="1">
-        <v>5.3545068993506399</v>
+        <v>2.0861952110389601</v>
       </c>
       <c r="C21" s="1">
-        <v>5.4089874188311597</v>
+        <v>2.2295008116883102</v>
       </c>
       <c r="D21" s="1">
-        <v>5.4970535714285704</v>
+        <v>2.1416883116883101</v>
       </c>
       <c r="E21" s="1">
-        <v>5.4455884740259703</v>
+        <v>2.1707061688311602</v>
       </c>
       <c r="F21" s="1">
-        <v>5.4997605519480501</v>
+        <v>2.2177130681818098</v>
       </c>
       <c r="G21" s="1">
-        <v>5.4367857142857101</v>
+        <v>2.1811566558441502</v>
       </c>
       <c r="H21" s="1">
-        <v>5.4395028409090802</v>
+        <v>2.0572098214285699</v>
       </c>
       <c r="I21" s="1">
-        <v>5.5414123376623303</v>
+        <v>2.2027962662337601</v>
       </c>
       <c r="J21" s="1">
-        <v>5.1316213474025902</v>
+        <v>2.1981107954545398</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
-        <v>4.81065543831168</v>
+        <v>4.5917816558441498</v>
       </c>
       <c r="B22" s="1">
-        <v>5.1288961038960998</v>
+        <v>4.5945556006493504</v>
       </c>
       <c r="C22" s="1">
-        <v>5.0258380681818098</v>
+        <v>4.7019825487012898</v>
       </c>
       <c r="D22" s="1">
-        <v>5.0245515422077904</v>
+        <v>4.60002232142857</v>
       </c>
       <c r="E22" s="1">
-        <v>5.0757081980519496</v>
+        <v>4.7393344155844099</v>
       </c>
       <c r="F22" s="1">
-        <v>4.9748823051948001</v>
+        <v>4.6667167207792097</v>
       </c>
       <c r="G22" s="1">
-        <v>5.1882548701298701</v>
+        <v>4.4920880681818103</v>
       </c>
       <c r="H22" s="1">
-        <v>5.1366659902597398</v>
+        <v>4.5418486201298602</v>
       </c>
       <c r="I22" s="1">
-        <v>5.0038474025974002</v>
+        <v>4.4995616883116902</v>
       </c>
       <c r="J22" s="1">
-        <v>5.0689224837662303</v>
+        <v>4.73885551948052</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
-        <v>5.8145758928571398</v>
+        <v>5.5341112012986997</v>
       </c>
       <c r="B23" s="1">
-        <v>5.9663920454545396</v>
+        <v>5.3545068993506399</v>
       </c>
       <c r="C23" s="1">
-        <v>5.5674594155844099</v>
+        <v>5.4089874188311597</v>
       </c>
       <c r="D23" s="1">
-        <v>5.7809983766233701</v>
+        <v>5.4970535714285704</v>
       </c>
       <c r="E23" s="1">
-        <v>5.3587073863636299</v>
+        <v>5.4455884740259703</v>
       </c>
       <c r="F23" s="1">
-        <v>5.6251359577922004</v>
+        <v>5.4997605519480501</v>
       </c>
       <c r="G23" s="1">
-        <v>5.9323579545454503</v>
+        <v>5.4367857142857101</v>
       </c>
       <c r="H23" s="1">
-        <v>5.3278672889610297</v>
+        <v>5.4395028409090802</v>
       </c>
       <c r="I23" s="1">
-        <v>5.5229646915584398</v>
+        <v>5.5414123376623303</v>
       </c>
       <c r="J23" s="1">
-        <v>5.8661404220779199</v>
+        <v>5.1316213474025902</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
-        <v>4.5626237824675302</v>
+        <v>4.81065543831168</v>
       </c>
       <c r="B24" s="1">
-        <v>5.94356331168831</v>
+        <v>5.1288961038960998</v>
       </c>
       <c r="C24" s="1">
-        <v>6.4157102272727196</v>
+        <v>5.0258380681818098</v>
       </c>
       <c r="D24" s="1">
-        <v>5.7926176948051902</v>
+        <v>5.0245515422077904</v>
       </c>
       <c r="E24" s="1">
-        <v>5.9248254870129804</v>
+        <v>5.0757081980519496</v>
       </c>
       <c r="F24" s="1">
-        <v>6.3800060876623297</v>
+        <v>4.9748823051948001</v>
       </c>
       <c r="G24" s="1">
-        <v>6.3701034902597398</v>
+        <v>5.1882548701298701</v>
       </c>
       <c r="H24" s="1">
-        <v>6.0724188311688296</v>
+        <v>5.1366659902597398</v>
       </c>
       <c r="I24" s="1">
-        <v>5.69140625</v>
+        <v>5.0038474025974002</v>
       </c>
       <c r="J24" s="1">
-        <v>6.59453327922078</v>
+        <v>5.0689224837662303</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
+        <v>5.8145758928571398</v>
+      </c>
+      <c r="B25" s="1">
+        <v>5.9663920454545396</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5.5674594155844099</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5.7809983766233701</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5.3587073863636299</v>
+      </c>
+      <c r="F25" s="1">
+        <v>5.6251359577922004</v>
+      </c>
+      <c r="G25" s="1">
+        <v>5.9323579545454503</v>
+      </c>
+      <c r="H25" s="1">
+        <v>5.3278672889610297</v>
+      </c>
+      <c r="I25" s="1">
+        <v>5.5229646915584398</v>
+      </c>
+      <c r="J25" s="1">
+        <v>5.8661404220779199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A26" s="1">
+        <v>4.5626237824675302</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5.94356331168831</v>
+      </c>
+      <c r="C26" s="1">
+        <v>6.4157102272727196</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5.7926176948051902</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5.9248254870129804</v>
+      </c>
+      <c r="F26" s="1">
+        <v>6.3800060876623297</v>
+      </c>
+      <c r="G26" s="1">
+        <v>6.3701034902597398</v>
+      </c>
+      <c r="H26" s="1">
+        <v>6.0724188311688296</v>
+      </c>
+      <c r="I26" s="1">
+        <v>5.69140625</v>
+      </c>
+      <c r="J26" s="1">
+        <v>6.59453327922078</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A27" s="1">
         <v>2.89396103896103</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B27" s="1">
         <v>2.8706209415584398</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C27" s="1">
         <v>2.91723417207792</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D27" s="1">
         <v>2.8703307629870101</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E27" s="1">
         <v>2.7576501623376601</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F27" s="1">
         <v>2.9595353084415499</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G27" s="1">
         <v>2.8679200487012899</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H27" s="1">
         <v>2.7958218344155799</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I27" s="1">
         <v>2.8814610389610298</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J27" s="1">
         <v>2.7844460227272698</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>